<commit_message>
Assignment 6 - Interpolated the dataset
</commit_message>
<xml_diff>
--- a/Assignment 6 CIELAB/Illuminant Data.xlsx
+++ b/Assignment 6 CIELAB/Illuminant Data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spfpci/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratheepkumarc/Documents/Development/Matlab/Principles-of-Color-Science/Assignment 6 CIELAB/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F430657-AAA0-724F-9D55-B0CC75637C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="3060" windowWidth="20960" windowHeight="8920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -91,6 +92,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -358,11 +362,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99:F108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>